<commit_message>
Fixed issues and added REMOVE action test
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Project_link_samples_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Project_link_samples_vtest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309FBD2F-0125-184C-87B1-C808B8921B53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E766D160-75DA-204C-8981-AF9203887171}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27760" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectLinkSamples" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Project link samples Template</t>
   </si>
@@ -81,12 +81,21 @@
   <si>
     <t>CONTAINER4PROJECTLINKSAMPLES2</t>
   </si>
+  <si>
+    <t>ProjectTest3</t>
+  </si>
+  <si>
+    <t>SampleTestForUnlink</t>
+  </si>
+  <si>
+    <t>CONTAINER4PROJECTLINKSAMPLES3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -147,6 +156,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -201,10 +215,10 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,8 +607,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="6" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="2" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="5" max="6" width="22.33203125" customWidth="1"/>
     <col min="7" max="26" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -699,15 +715,23 @@
       <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="A12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -715,7 +739,7 @@
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -723,7 +747,7 @@
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -731,7 +755,7 @@
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -739,7 +763,7 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -747,7 +771,7 @@
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -755,7 +779,7 @@
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -763,7 +787,7 @@
       <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -771,7 +795,7 @@
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -779,7 +803,7 @@
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -787,7 +811,7 @@
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -795,7 +819,7 @@
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -803,7 +827,7 @@
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -811,7 +835,7 @@
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -819,7 +843,7 @@
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -827,7 +851,7 @@
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -835,7 +859,7 @@
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -843,7 +867,7 @@
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -851,7 +875,7 @@
       <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -859,7 +883,7 @@
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -867,7 +891,7 @@
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -875,7 +899,7 @@
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -883,7 +907,7 @@
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -891,7 +915,7 @@
       <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -899,7 +923,7 @@
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="8"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -907,7 +931,7 @@
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="8"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -915,7 +939,7 @@
       <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="8"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -923,7 +947,7 @@
       <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -931,7 +955,7 @@
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -939,7 +963,7 @@
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
+      <c r="A42" s="13"/>
       <c r="B42" s="8"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
@@ -947,7 +971,7 @@
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="8"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -955,7 +979,7 @@
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="8"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -963,7 +987,7 @@
       <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="8"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -971,7 +995,7 @@
       <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="8"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
@@ -979,7 +1003,7 @@
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -987,7 +1011,7 @@
       <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
@@ -995,7 +1019,7 @@
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="8"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -1003,7 +1027,7 @@
       <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
@@ -1011,7 +1035,7 @@
       <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -1019,7 +1043,7 @@
       <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
+      <c r="A52" s="13"/>
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -1027,7 +1051,7 @@
       <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
+      <c r="A53" s="13"/>
       <c r="B53" s="8"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -1035,7 +1059,7 @@
       <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
+      <c r="A54" s="13"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -1043,7 +1067,7 @@
       <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="8"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -1051,7 +1075,7 @@
       <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
+      <c r="A56" s="13"/>
       <c r="B56" s="8"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -1059,7 +1083,7 @@
       <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
+      <c r="A57" s="13"/>
       <c r="B57" s="8"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -1067,7 +1091,7 @@
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="8"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -1075,7 +1099,7 @@
       <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
+      <c r="A59" s="13"/>
       <c r="B59" s="8"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -1083,7 +1107,7 @@
       <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
+      <c r="A60" s="13"/>
       <c r="B60" s="8"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -1091,7 +1115,7 @@
       <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="8"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
@@ -1099,7 +1123,7 @@
       <c r="F61" s="9"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4"/>
+      <c r="A62" s="13"/>
       <c r="B62" s="8"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
@@ -1107,7 +1131,7 @@
       <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4"/>
+      <c r="A63" s="13"/>
       <c r="B63" s="8"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
@@ -1115,7 +1139,7 @@
       <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4"/>
+      <c r="A64" s="13"/>
       <c r="B64" s="8"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
@@ -1123,7 +1147,7 @@
       <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="4"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="8"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
@@ -1131,7 +1155,7 @@
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4"/>
+      <c r="A66" s="13"/>
       <c r="B66" s="8"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
@@ -1139,7 +1163,7 @@
       <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4"/>
+      <c r="A67" s="13"/>
       <c r="B67" s="8"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
@@ -1147,7 +1171,7 @@
       <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4"/>
+      <c r="A68" s="13"/>
       <c r="B68" s="8"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
@@ -1155,7 +1179,7 @@
       <c r="F68" s="9"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4"/>
+      <c r="A69" s="13"/>
       <c r="B69" s="8"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
@@ -1163,7 +1187,7 @@
       <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
+      <c r="A70" s="13"/>
       <c r="B70" s="8"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
@@ -1171,7 +1195,7 @@
       <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4"/>
+      <c r="A71" s="13"/>
       <c r="B71" s="8"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
@@ -1179,7 +1203,7 @@
       <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
+      <c r="A72" s="13"/>
       <c r="B72" s="8"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
@@ -1187,7 +1211,7 @@
       <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
+      <c r="A73" s="13"/>
       <c r="B73" s="8"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
@@ -1195,7 +1219,7 @@
       <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
+      <c r="A74" s="13"/>
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
@@ -1203,7 +1227,7 @@
       <c r="F74" s="9"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
+      <c r="A75" s="13"/>
       <c r="B75" s="8"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
@@ -1211,7 +1235,7 @@
       <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
+      <c r="A76" s="13"/>
       <c r="B76" s="8"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
@@ -1219,7 +1243,7 @@
       <c r="F76" s="9"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4"/>
+      <c r="A77" s="13"/>
       <c r="B77" s="8"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
@@ -1227,7 +1251,7 @@
       <c r="F77" s="9"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="4"/>
+      <c r="A78" s="13"/>
       <c r="B78" s="8"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
@@ -1235,7 +1259,7 @@
       <c r="F78" s="9"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="4"/>
+      <c r="A79" s="13"/>
       <c r="B79" s="8"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
@@ -1243,7 +1267,7 @@
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4"/>
+      <c r="A80" s="13"/>
       <c r="B80" s="8"/>
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
@@ -1251,7 +1275,7 @@
       <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4"/>
+      <c r="A81" s="13"/>
       <c r="B81" s="8"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
@@ -1259,7 +1283,7 @@
       <c r="F81" s="9"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4"/>
+      <c r="A82" s="13"/>
       <c r="B82" s="8"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
@@ -1267,7 +1291,7 @@
       <c r="F82" s="9"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="4"/>
+      <c r="A83" s="13"/>
       <c r="B83" s="8"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
@@ -1275,7 +1299,7 @@
       <c r="F83" s="9"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="4"/>
+      <c r="A84" s="13"/>
       <c r="B84" s="8"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
@@ -1283,7 +1307,7 @@
       <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="4"/>
+      <c r="A85" s="13"/>
       <c r="B85" s="8"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
@@ -1291,7 +1315,7 @@
       <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="4"/>
+      <c r="A86" s="13"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
@@ -1299,7 +1323,7 @@
       <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="4"/>
+      <c r="A87" s="13"/>
       <c r="B87" s="8"/>
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
@@ -1307,7 +1331,7 @@
       <c r="F87" s="9"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="4"/>
+      <c r="A88" s="13"/>
       <c r="B88" s="8"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
@@ -1315,7 +1339,7 @@
       <c r="F88" s="9"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="4"/>
+      <c r="A89" s="13"/>
       <c r="B89" s="8"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
@@ -1323,7 +1347,7 @@
       <c r="F89" s="9"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="4"/>
+      <c r="A90" s="13"/>
       <c r="B90" s="8"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
@@ -1331,7 +1355,7 @@
       <c r="F90" s="9"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="4"/>
+      <c r="A91" s="13"/>
       <c r="B91" s="8"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
@@ -1339,7 +1363,7 @@
       <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="4"/>
+      <c r="A92" s="13"/>
       <c r="B92" s="8"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
@@ -1347,7 +1371,7 @@
       <c r="F92" s="9"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="4"/>
+      <c r="A93" s="13"/>
       <c r="B93" s="8"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
@@ -1355,7 +1379,7 @@
       <c r="F93" s="9"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="4"/>
+      <c r="A94" s="13"/>
       <c r="B94" s="8"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
@@ -1363,7 +1387,7 @@
       <c r="F94" s="9"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="4"/>
+      <c r="A95" s="13"/>
       <c r="B95" s="8"/>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
@@ -1371,7 +1395,7 @@
       <c r="F95" s="9"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="4"/>
+      <c r="A96" s="13"/>
       <c r="B96" s="8"/>
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
@@ -1379,7 +1403,7 @@
       <c r="F96" s="9"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
+      <c r="A97" s="13"/>
       <c r="B97" s="8"/>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
@@ -1387,7 +1411,7 @@
       <c r="F97" s="9"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="4"/>
+      <c r="A98" s="13"/>
       <c r="B98" s="8"/>
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
@@ -1395,7 +1419,7 @@
       <c r="F98" s="9"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="4"/>
+      <c r="A99" s="13"/>
       <c r="B99" s="8"/>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
@@ -1403,7 +1427,7 @@
       <c r="F99" s="9"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="4"/>
+      <c r="A100" s="13"/>
       <c r="B100" s="8"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
@@ -1411,7 +1435,7 @@
       <c r="F100" s="9"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="4"/>
+      <c r="A101" s="13"/>
       <c r="B101" s="8"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
@@ -1419,7 +1443,7 @@
       <c r="F101" s="9"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="4"/>
+      <c r="A102" s="13"/>
       <c r="B102" s="8"/>
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
@@ -1427,7 +1451,7 @@
       <c r="F102" s="9"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
+      <c r="A103" s="13"/>
       <c r="B103" s="8"/>
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
@@ -1435,7 +1459,7 @@
       <c r="F103" s="9"/>
     </row>
     <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="4"/>
+      <c r="A104" s="13"/>
       <c r="B104" s="8"/>
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
@@ -1443,7 +1467,7 @@
       <c r="F104" s="9"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="4"/>
+      <c r="A105" s="13"/>
       <c r="B105" s="8"/>
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
@@ -1451,7 +1475,7 @@
       <c r="F105" s="9"/>
     </row>
     <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="4"/>
+      <c r="A106" s="13"/>
       <c r="B106" s="8"/>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
@@ -1459,7 +1483,7 @@
       <c r="F106" s="9"/>
     </row>
     <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="4"/>
+      <c r="A107" s="13"/>
       <c r="B107" s="8"/>
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
@@ -1467,7 +1491,7 @@
       <c r="F107" s="9"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="4"/>
+      <c r="A108" s="13"/>
       <c r="B108" s="8"/>
       <c r="C108" s="9"/>
       <c r="D108" s="9"/>
@@ -1475,932 +1499,932 @@
       <c r="F108" s="9"/>
     </row>
     <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="4"/>
-      <c r="B109" s="12"/>
-      <c r="C109" s="13"/>
-      <c r="D109" s="13"/>
-      <c r="E109" s="13"/>
-      <c r="F109" s="13"/>
+      <c r="A109" s="13"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
     </row>
     <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="4"/>
-      <c r="B110" s="12"/>
-      <c r="C110" s="13"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="13"/>
-      <c r="F110" s="13"/>
+      <c r="A110" s="13"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
     </row>
     <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="4"/>
-      <c r="B111" s="12"/>
-      <c r="C111" s="13"/>
-      <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
+      <c r="A111" s="13"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
     </row>
     <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="4"/>
-      <c r="B112" s="12"/>
-      <c r="C112" s="13"/>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
+      <c r="A112" s="13"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="12"/>
     </row>
     <row r="113" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="4"/>
-      <c r="B113" s="12"/>
-      <c r="C113" s="13"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="13"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
     </row>
     <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="4"/>
-      <c r="B114" s="12"/>
-      <c r="C114" s="13"/>
-      <c r="D114" s="13"/>
-      <c r="E114" s="13"/>
-      <c r="F114" s="13"/>
+      <c r="A114" s="13"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
     </row>
     <row r="115" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="4"/>
-      <c r="B115" s="12"/>
-      <c r="C115" s="13"/>
-      <c r="D115" s="13"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="13"/>
+      <c r="A115" s="13"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
     </row>
     <row r="116" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="4"/>
-      <c r="B116" s="12"/>
-      <c r="C116" s="13"/>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="4"/>
-      <c r="B117" s="12"/>
-      <c r="C117" s="13"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
     </row>
     <row r="118" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="4"/>
-      <c r="B118" s="12"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="13"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="12"/>
     </row>
     <row r="119" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="4"/>
-      <c r="B119" s="12"/>
-      <c r="C119" s="13"/>
-      <c r="D119" s="13"/>
-      <c r="E119" s="13"/>
-      <c r="F119" s="13"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
     </row>
     <row r="120" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="4"/>
-      <c r="B120" s="12"/>
-      <c r="C120" s="13"/>
-      <c r="D120" s="13"/>
-      <c r="E120" s="13"/>
-      <c r="F120" s="13"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="4"/>
-      <c r="B121" s="12"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="13"/>
-      <c r="E121" s="13"/>
-      <c r="F121" s="13"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
     </row>
     <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="4"/>
-      <c r="B122" s="12"/>
-      <c r="C122" s="13"/>
-      <c r="D122" s="13"/>
-      <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
     </row>
     <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="4"/>
-      <c r="B123" s="12"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="13"/>
-      <c r="E123" s="13"/>
-      <c r="F123" s="13"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
     </row>
     <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="4"/>
-      <c r="B124" s="12"/>
-      <c r="C124" s="13"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
     </row>
     <row r="125" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="4"/>
-      <c r="B125" s="12"/>
-      <c r="C125" s="13"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
     </row>
     <row r="126" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="4"/>
-      <c r="B126" s="12"/>
-      <c r="C126" s="13"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
     </row>
     <row r="127" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="4"/>
-      <c r="B127" s="12"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
     </row>
     <row r="128" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="4"/>
-      <c r="B128" s="12"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="12"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
+      <c r="F128" s="12"/>
     </row>
     <row r="129" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="4"/>
-      <c r="B129" s="12"/>
-      <c r="C129" s="13"/>
-      <c r="D129" s="13"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
     </row>
     <row r="130" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="4"/>
-      <c r="B130" s="12"/>
-      <c r="C130" s="13"/>
-      <c r="D130" s="13"/>
-      <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
     </row>
     <row r="131" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="4"/>
-      <c r="B131" s="12"/>
-      <c r="C131" s="13"/>
-      <c r="D131" s="13"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
+      <c r="A131" s="13"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="12"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12"/>
     </row>
     <row r="132" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="4"/>
-      <c r="B132" s="12"/>
-      <c r="C132" s="13"/>
-      <c r="D132" s="13"/>
-      <c r="E132" s="13"/>
-      <c r="F132" s="13"/>
+      <c r="A132" s="13"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
     </row>
     <row r="133" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="4"/>
-      <c r="B133" s="12"/>
-      <c r="C133" s="13"/>
-      <c r="D133" s="13"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
+      <c r="A133" s="13"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="12"/>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
+      <c r="F133" s="12"/>
     </row>
     <row r="134" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="4"/>
-      <c r="B134" s="12"/>
-      <c r="C134" s="13"/>
-      <c r="D134" s="13"/>
-      <c r="E134" s="13"/>
-      <c r="F134" s="13"/>
+      <c r="A134" s="13"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
     </row>
     <row r="135" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="4"/>
-      <c r="B135" s="12"/>
-      <c r="C135" s="13"/>
-      <c r="D135" s="13"/>
-      <c r="E135" s="13"/>
-      <c r="F135" s="13"/>
+      <c r="A135" s="13"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
     </row>
     <row r="136" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="4"/>
-      <c r="B136" s="12"/>
-      <c r="C136" s="13"/>
-      <c r="D136" s="13"/>
-      <c r="E136" s="13"/>
-      <c r="F136" s="13"/>
+      <c r="A136" s="13"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
+      <c r="F136" s="12"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="4"/>
-      <c r="B137" s="12"/>
-      <c r="C137" s="13"/>
-      <c r="D137" s="13"/>
-      <c r="E137" s="13"/>
-      <c r="F137" s="13"/>
+      <c r="A137" s="13"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
     </row>
     <row r="138" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="4"/>
-      <c r="B138" s="12"/>
-      <c r="C138" s="13"/>
-      <c r="D138" s="13"/>
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
+      <c r="A138" s="13"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
     </row>
     <row r="139" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="4"/>
-      <c r="B139" s="12"/>
-      <c r="C139" s="13"/>
-      <c r="D139" s="13"/>
-      <c r="E139" s="13"/>
-      <c r="F139" s="13"/>
+      <c r="A139" s="13"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="12"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
     </row>
     <row r="140" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="4"/>
-      <c r="B140" s="12"/>
-      <c r="C140" s="13"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
+      <c r="A140" s="13"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
     </row>
     <row r="141" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="4"/>
-      <c r="B141" s="4"/>
+      <c r="A141" s="13"/>
+      <c r="B141" s="8"/>
     </row>
     <row r="142" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="4"/>
-      <c r="B142" s="4"/>
+      <c r="A142" s="13"/>
+      <c r="B142" s="8"/>
     </row>
     <row r="143" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="4"/>
-      <c r="B143" s="4"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="8"/>
     </row>
     <row r="144" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="4"/>
-      <c r="B144" s="4"/>
+      <c r="A144" s="13"/>
+      <c r="B144" s="8"/>
     </row>
     <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="4"/>
-      <c r="B145" s="4"/>
+      <c r="A145" s="13"/>
+      <c r="B145" s="8"/>
     </row>
     <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="4"/>
-      <c r="B146" s="4"/>
+      <c r="A146" s="13"/>
+      <c r="B146" s="8"/>
     </row>
     <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="4"/>
-      <c r="B147" s="4"/>
+      <c r="A147" s="13"/>
+      <c r="B147" s="8"/>
     </row>
     <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="4"/>
-      <c r="B148" s="4"/>
+      <c r="A148" s="13"/>
+      <c r="B148" s="8"/>
     </row>
     <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="4"/>
-      <c r="B149" s="4"/>
+      <c r="A149" s="13"/>
+      <c r="B149" s="8"/>
     </row>
     <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="4"/>
-      <c r="B150" s="4"/>
+      <c r="A150" s="13"/>
+      <c r="B150" s="8"/>
     </row>
     <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
+      <c r="A151" s="13"/>
+      <c r="B151" s="8"/>
     </row>
     <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="4"/>
-      <c r="B152" s="4"/>
+      <c r="A152" s="13"/>
+      <c r="B152" s="8"/>
     </row>
     <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="4"/>
-      <c r="B153" s="4"/>
+      <c r="A153" s="13"/>
+      <c r="B153" s="8"/>
     </row>
     <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="4"/>
-      <c r="B154" s="4"/>
+      <c r="A154" s="13"/>
+      <c r="B154" s="8"/>
     </row>
     <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="4"/>
-      <c r="B155" s="4"/>
+      <c r="A155" s="13"/>
+      <c r="B155" s="8"/>
     </row>
     <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="4"/>
-      <c r="B156" s="4"/>
+      <c r="A156" s="13"/>
+      <c r="B156" s="8"/>
     </row>
     <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="4"/>
-      <c r="B157" s="4"/>
+      <c r="A157" s="13"/>
+      <c r="B157" s="8"/>
     </row>
     <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="4"/>
-      <c r="B158" s="4"/>
+      <c r="A158" s="13"/>
+      <c r="B158" s="8"/>
     </row>
     <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="4"/>
-      <c r="B159" s="4"/>
+      <c r="A159" s="13"/>
+      <c r="B159" s="8"/>
     </row>
     <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="4"/>
-      <c r="B160" s="4"/>
+      <c r="A160" s="13"/>
+      <c r="B160" s="8"/>
     </row>
     <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="4"/>
-      <c r="B161" s="4"/>
+      <c r="A161" s="13"/>
+      <c r="B161" s="8"/>
     </row>
     <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="4"/>
-      <c r="B162" s="4"/>
+      <c r="A162" s="13"/>
+      <c r="B162" s="8"/>
     </row>
     <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="4"/>
-      <c r="B163" s="4"/>
+      <c r="A163" s="13"/>
+      <c r="B163" s="8"/>
     </row>
     <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="4"/>
-      <c r="B164" s="4"/>
+      <c r="A164" s="13"/>
+      <c r="B164" s="8"/>
     </row>
     <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="4"/>
-      <c r="B165" s="4"/>
+      <c r="A165" s="13"/>
+      <c r="B165" s="8"/>
     </row>
     <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="4"/>
-      <c r="B166" s="4"/>
+      <c r="A166" s="13"/>
+      <c r="B166" s="8"/>
     </row>
     <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="4"/>
-      <c r="B167" s="4"/>
+      <c r="A167" s="13"/>
+      <c r="B167" s="8"/>
     </row>
     <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="4"/>
-      <c r="B168" s="4"/>
+      <c r="A168" s="13"/>
+      <c r="B168" s="8"/>
     </row>
     <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="4"/>
-      <c r="B169" s="4"/>
+      <c r="A169" s="13"/>
+      <c r="B169" s="8"/>
     </row>
     <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="4"/>
-      <c r="B170" s="4"/>
+      <c r="A170" s="13"/>
+      <c r="B170" s="8"/>
     </row>
     <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="4"/>
-      <c r="B171" s="4"/>
+      <c r="A171" s="13"/>
+      <c r="B171" s="8"/>
     </row>
     <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="4"/>
-      <c r="B172" s="4"/>
+      <c r="A172" s="13"/>
+      <c r="B172" s="8"/>
     </row>
     <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="4"/>
-      <c r="B173" s="4"/>
+      <c r="A173" s="13"/>
+      <c r="B173" s="8"/>
     </row>
     <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="4"/>
-      <c r="B174" s="4"/>
+      <c r="A174" s="13"/>
+      <c r="B174" s="8"/>
     </row>
     <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="4"/>
-      <c r="B175" s="4"/>
+      <c r="A175" s="13"/>
+      <c r="B175" s="8"/>
     </row>
     <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="4"/>
-      <c r="B176" s="4"/>
+      <c r="A176" s="13"/>
+      <c r="B176" s="8"/>
     </row>
     <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="4"/>
-      <c r="B177" s="4"/>
+      <c r="A177" s="13"/>
+      <c r="B177" s="8"/>
     </row>
     <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="4"/>
-      <c r="B178" s="4"/>
+      <c r="A178" s="13"/>
+      <c r="B178" s="8"/>
     </row>
     <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="4"/>
-      <c r="B179" s="4"/>
+      <c r="A179" s="13"/>
+      <c r="B179" s="8"/>
     </row>
     <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="4"/>
-      <c r="B180" s="4"/>
+      <c r="A180" s="13"/>
+      <c r="B180" s="8"/>
     </row>
     <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="4"/>
-      <c r="B181" s="4"/>
+      <c r="A181" s="13"/>
+      <c r="B181" s="8"/>
     </row>
     <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="4"/>
-      <c r="B182" s="4"/>
+      <c r="A182" s="13"/>
+      <c r="B182" s="8"/>
     </row>
     <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="4"/>
-      <c r="B183" s="4"/>
+      <c r="A183" s="13"/>
+      <c r="B183" s="8"/>
     </row>
     <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="4"/>
-      <c r="B184" s="4"/>
+      <c r="A184" s="13"/>
+      <c r="B184" s="8"/>
     </row>
     <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="4"/>
-      <c r="B185" s="4"/>
+      <c r="A185" s="13"/>
+      <c r="B185" s="8"/>
     </row>
     <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="4"/>
-      <c r="B186" s="4"/>
+      <c r="A186" s="13"/>
+      <c r="B186" s="8"/>
     </row>
     <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="4"/>
-      <c r="B187" s="4"/>
+      <c r="A187" s="13"/>
+      <c r="B187" s="8"/>
     </row>
     <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="4"/>
-      <c r="B188" s="4"/>
+      <c r="A188" s="13"/>
+      <c r="B188" s="8"/>
     </row>
     <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="4"/>
-      <c r="B189" s="4"/>
+      <c r="A189" s="13"/>
+      <c r="B189" s="8"/>
     </row>
     <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="4"/>
-      <c r="B190" s="4"/>
+      <c r="A190" s="13"/>
+      <c r="B190" s="8"/>
     </row>
     <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="4"/>
-      <c r="B191" s="4"/>
+      <c r="A191" s="13"/>
+      <c r="B191" s="8"/>
     </row>
     <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="4"/>
-      <c r="B192" s="4"/>
+      <c r="A192" s="13"/>
+      <c r="B192" s="8"/>
     </row>
     <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="4"/>
-      <c r="B193" s="4"/>
+      <c r="A193" s="13"/>
+      <c r="B193" s="8"/>
     </row>
     <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="4"/>
-      <c r="B194" s="4"/>
+      <c r="A194" s="13"/>
+      <c r="B194" s="8"/>
     </row>
     <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="4"/>
-      <c r="B195" s="4"/>
+      <c r="A195" s="13"/>
+      <c r="B195" s="8"/>
     </row>
     <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="4"/>
-      <c r="B196" s="4"/>
+      <c r="A196" s="13"/>
+      <c r="B196" s="8"/>
     </row>
     <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="4"/>
-      <c r="B197" s="4"/>
+      <c r="A197" s="13"/>
+      <c r="B197" s="8"/>
     </row>
     <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="4"/>
-      <c r="B198" s="4"/>
+      <c r="A198" s="13"/>
+      <c r="B198" s="8"/>
     </row>
     <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="4"/>
-      <c r="B199" s="4"/>
+      <c r="A199" s="13"/>
+      <c r="B199" s="8"/>
     </row>
     <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A200" s="4"/>
-      <c r="B200" s="4"/>
+      <c r="A200" s="13"/>
+      <c r="B200" s="8"/>
     </row>
     <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="4"/>
-      <c r="B201" s="4"/>
+      <c r="A201" s="13"/>
+      <c r="B201" s="8"/>
     </row>
     <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="4"/>
-      <c r="B202" s="4"/>
+      <c r="A202" s="13"/>
+      <c r="B202" s="8"/>
     </row>
     <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="4"/>
-      <c r="B203" s="4"/>
+      <c r="A203" s="13"/>
+      <c r="B203" s="8"/>
     </row>
     <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="4"/>
-      <c r="B204" s="4"/>
+      <c r="A204" s="13"/>
+      <c r="B204" s="8"/>
     </row>
     <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="4"/>
-      <c r="B205" s="4"/>
+      <c r="A205" s="13"/>
+      <c r="B205" s="8"/>
     </row>
     <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A206" s="4"/>
-      <c r="B206" s="4"/>
+      <c r="A206" s="13"/>
+      <c r="B206" s="8"/>
     </row>
     <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="4"/>
-      <c r="B207" s="4"/>
+      <c r="A207" s="13"/>
+      <c r="B207" s="8"/>
     </row>
     <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A208" s="4"/>
-      <c r="B208" s="4"/>
+      <c r="A208" s="13"/>
+      <c r="B208" s="8"/>
     </row>
     <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A209" s="4"/>
-      <c r="B209" s="4"/>
+      <c r="A209" s="13"/>
+      <c r="B209" s="8"/>
     </row>
     <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="4"/>
-      <c r="B210" s="4"/>
+      <c r="A210" s="13"/>
+      <c r="B210" s="8"/>
     </row>
     <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="4"/>
-      <c r="B211" s="4"/>
+      <c r="A211" s="13"/>
+      <c r="B211" s="8"/>
     </row>
     <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="4"/>
-      <c r="B212" s="4"/>
+      <c r="A212" s="13"/>
+      <c r="B212" s="8"/>
     </row>
     <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="4"/>
-      <c r="B213" s="4"/>
+      <c r="A213" s="13"/>
+      <c r="B213" s="8"/>
     </row>
     <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A214" s="4"/>
-      <c r="B214" s="4"/>
+      <c r="A214" s="13"/>
+      <c r="B214" s="8"/>
     </row>
     <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A215" s="4"/>
-      <c r="B215" s="4"/>
+      <c r="A215" s="13"/>
+      <c r="B215" s="8"/>
     </row>
     <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A216" s="4"/>
-      <c r="B216" s="4"/>
+      <c r="A216" s="13"/>
+      <c r="B216" s="8"/>
     </row>
     <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A217" s="4"/>
-      <c r="B217" s="4"/>
+      <c r="A217" s="13"/>
+      <c r="B217" s="8"/>
     </row>
     <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A218" s="4"/>
-      <c r="B218" s="4"/>
+      <c r="A218" s="13"/>
+      <c r="B218" s="8"/>
     </row>
     <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A219" s="4"/>
-      <c r="B219" s="4"/>
+      <c r="A219" s="13"/>
+      <c r="B219" s="8"/>
     </row>
     <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="4"/>
-      <c r="B220" s="4"/>
+      <c r="A220" s="13"/>
+      <c r="B220" s="8"/>
     </row>
     <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A221" s="4"/>
-      <c r="B221" s="4"/>
+      <c r="A221" s="13"/>
+      <c r="B221" s="8"/>
     </row>
     <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A222" s="4"/>
-      <c r="B222" s="4"/>
+      <c r="A222" s="13"/>
+      <c r="B222" s="8"/>
     </row>
     <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A223" s="4"/>
-      <c r="B223" s="4"/>
+      <c r="A223" s="13"/>
+      <c r="B223" s="8"/>
     </row>
     <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A224" s="4"/>
-      <c r="B224" s="4"/>
+      <c r="A224" s="13"/>
+      <c r="B224" s="8"/>
     </row>
     <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A225" s="4"/>
-      <c r="B225" s="4"/>
+      <c r="A225" s="13"/>
+      <c r="B225" s="8"/>
     </row>
     <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A226" s="4"/>
-      <c r="B226" s="4"/>
+      <c r="A226" s="13"/>
+      <c r="B226" s="8"/>
     </row>
     <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A227" s="4"/>
-      <c r="B227" s="4"/>
+      <c r="A227" s="13"/>
+      <c r="B227" s="8"/>
     </row>
     <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A228" s="4"/>
-      <c r="B228" s="4"/>
+      <c r="A228" s="13"/>
+      <c r="B228" s="8"/>
     </row>
     <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A229" s="4"/>
-      <c r="B229" s="4"/>
+      <c r="A229" s="13"/>
+      <c r="B229" s="8"/>
     </row>
     <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A230" s="4"/>
-      <c r="B230" s="4"/>
+      <c r="A230" s="13"/>
+      <c r="B230" s="8"/>
     </row>
     <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="4"/>
-      <c r="B231" s="4"/>
+      <c r="A231" s="13"/>
+      <c r="B231" s="8"/>
     </row>
     <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A232" s="4"/>
-      <c r="B232" s="4"/>
+      <c r="A232" s="13"/>
+      <c r="B232" s="8"/>
     </row>
     <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A233" s="4"/>
-      <c r="B233" s="4"/>
+      <c r="A233" s="13"/>
+      <c r="B233" s="8"/>
     </row>
     <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A234" s="4"/>
-      <c r="B234" s="4"/>
+      <c r="A234" s="13"/>
+      <c r="B234" s="8"/>
     </row>
     <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A235" s="4"/>
-      <c r="B235" s="4"/>
+      <c r="A235" s="13"/>
+      <c r="B235" s="8"/>
     </row>
     <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="4"/>
-      <c r="B236" s="4"/>
+      <c r="A236" s="13"/>
+      <c r="B236" s="8"/>
     </row>
     <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A237" s="4"/>
-      <c r="B237" s="4"/>
+      <c r="A237" s="13"/>
+      <c r="B237" s="8"/>
     </row>
     <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A238" s="4"/>
-      <c r="B238" s="4"/>
+      <c r="A238" s="13"/>
+      <c r="B238" s="8"/>
     </row>
     <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A239" s="4"/>
-      <c r="B239" s="4"/>
+      <c r="A239" s="13"/>
+      <c r="B239" s="8"/>
     </row>
     <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A240" s="4"/>
-      <c r="B240" s="4"/>
+      <c r="A240" s="13"/>
+      <c r="B240" s="8"/>
     </row>
     <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A241" s="4"/>
-      <c r="B241" s="4"/>
+      <c r="A241" s="13"/>
+      <c r="B241" s="8"/>
     </row>
     <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A242" s="4"/>
-      <c r="B242" s="4"/>
+      <c r="A242" s="13"/>
+      <c r="B242" s="8"/>
     </row>
     <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A243" s="4"/>
-      <c r="B243" s="4"/>
+      <c r="A243" s="13"/>
+      <c r="B243" s="8"/>
     </row>
     <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A244" s="4"/>
-      <c r="B244" s="4"/>
+      <c r="A244" s="13"/>
+      <c r="B244" s="8"/>
     </row>
     <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A245" s="4"/>
-      <c r="B245" s="4"/>
+      <c r="A245" s="13"/>
+      <c r="B245" s="8"/>
     </row>
     <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A246" s="4"/>
-      <c r="B246" s="4"/>
+      <c r="A246" s="13"/>
+      <c r="B246" s="8"/>
     </row>
     <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A247" s="4"/>
-      <c r="B247" s="4"/>
+      <c r="A247" s="13"/>
+      <c r="B247" s="8"/>
     </row>
     <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A248" s="4"/>
-      <c r="B248" s="4"/>
+      <c r="A248" s="13"/>
+      <c r="B248" s="8"/>
     </row>
     <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A249" s="4"/>
-      <c r="B249" s="4"/>
+      <c r="A249" s="13"/>
+      <c r="B249" s="8"/>
     </row>
     <row r="250" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A250" s="4"/>
-      <c r="B250" s="4"/>
+      <c r="A250" s="13"/>
+      <c r="B250" s="8"/>
     </row>
     <row r="251" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A251" s="4"/>
-      <c r="B251" s="4"/>
+      <c r="A251" s="13"/>
+      <c r="B251" s="8"/>
     </row>
     <row r="252" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A252" s="4"/>
-      <c r="B252" s="4"/>
+      <c r="A252" s="13"/>
+      <c r="B252" s="8"/>
     </row>
     <row r="253" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A253" s="4"/>
-      <c r="B253" s="4"/>
+      <c r="A253" s="13"/>
+      <c r="B253" s="8"/>
     </row>
     <row r="254" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A254" s="4"/>
-      <c r="B254" s="4"/>
+      <c r="A254" s="13"/>
+      <c r="B254" s="8"/>
     </row>
     <row r="255" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A255" s="4"/>
-      <c r="B255" s="4"/>
+      <c r="A255" s="13"/>
+      <c r="B255" s="8"/>
     </row>
     <row r="256" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A256" s="4"/>
-      <c r="B256" s="4"/>
+      <c r="A256" s="13"/>
+      <c r="B256" s="8"/>
     </row>
     <row r="257" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A257" s="4"/>
-      <c r="B257" s="4"/>
+      <c r="A257" s="13"/>
+      <c r="B257" s="8"/>
     </row>
     <row r="258" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A258" s="4"/>
-      <c r="B258" s="4"/>
+      <c r="A258" s="13"/>
+      <c r="B258" s="8"/>
     </row>
     <row r="259" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A259" s="4"/>
-      <c r="B259" s="4"/>
+      <c r="A259" s="13"/>
+      <c r="B259" s="8"/>
     </row>
     <row r="260" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A260" s="4"/>
-      <c r="B260" s="4"/>
+      <c r="A260" s="13"/>
+      <c r="B260" s="8"/>
     </row>
     <row r="261" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A261" s="4"/>
-      <c r="B261" s="4"/>
+      <c r="A261" s="13"/>
+      <c r="B261" s="8"/>
     </row>
     <row r="262" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A262" s="4"/>
-      <c r="B262" s="4"/>
+      <c r="A262" s="13"/>
+      <c r="B262" s="8"/>
     </row>
     <row r="263" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A263" s="4"/>
-      <c r="B263" s="4"/>
+      <c r="A263" s="13"/>
+      <c r="B263" s="8"/>
     </row>
     <row r="264" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A264" s="4"/>
-      <c r="B264" s="4"/>
+      <c r="A264" s="13"/>
+      <c r="B264" s="8"/>
     </row>
     <row r="265" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A265" s="4"/>
-      <c r="B265" s="4"/>
+      <c r="A265" s="13"/>
+      <c r="B265" s="8"/>
     </row>
     <row r="266" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A266" s="4"/>
-      <c r="B266" s="4"/>
+      <c r="A266" s="13"/>
+      <c r="B266" s="8"/>
     </row>
     <row r="267" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A267" s="4"/>
-      <c r="B267" s="4"/>
+      <c r="A267" s="13"/>
+      <c r="B267" s="8"/>
     </row>
     <row r="268" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A268" s="4"/>
-      <c r="B268" s="4"/>
+      <c r="A268" s="13"/>
+      <c r="B268" s="8"/>
     </row>
     <row r="269" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A269" s="4"/>
-      <c r="B269" s="4"/>
+      <c r="A269" s="13"/>
+      <c r="B269" s="8"/>
     </row>
     <row r="270" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A270" s="4"/>
-      <c r="B270" s="4"/>
+      <c r="A270" s="13"/>
+      <c r="B270" s="8"/>
     </row>
     <row r="271" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A271" s="4"/>
-      <c r="B271" s="4"/>
+      <c r="A271" s="13"/>
+      <c r="B271" s="8"/>
     </row>
     <row r="272" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A272" s="4"/>
-      <c r="B272" s="4"/>
+      <c r="A272" s="13"/>
+      <c r="B272" s="8"/>
     </row>
     <row r="273" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A273" s="4"/>
-      <c r="B273" s="4"/>
+      <c r="A273" s="13"/>
+      <c r="B273" s="8"/>
     </row>
     <row r="274" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A274" s="4"/>
-      <c r="B274" s="4"/>
+      <c r="A274" s="13"/>
+      <c r="B274" s="8"/>
     </row>
     <row r="275" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A275" s="4"/>
-      <c r="B275" s="4"/>
+      <c r="A275" s="13"/>
+      <c r="B275" s="8"/>
     </row>
     <row r="276" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A276" s="4"/>
-      <c r="B276" s="4"/>
+      <c r="A276" s="13"/>
+      <c r="B276" s="8"/>
     </row>
     <row r="277" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A277" s="4"/>
-      <c r="B277" s="4"/>
+      <c r="A277" s="13"/>
+      <c r="B277" s="8"/>
     </row>
     <row r="278" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A278" s="4"/>
-      <c r="B278" s="4"/>
+      <c r="A278" s="13"/>
+      <c r="B278" s="8"/>
     </row>
     <row r="279" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A279" s="4"/>
-      <c r="B279" s="4"/>
+      <c r="A279" s="13"/>
+      <c r="B279" s="8"/>
     </row>
     <row r="280" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A280" s="4"/>
-      <c r="B280" s="4"/>
+      <c r="A280" s="13"/>
+      <c r="B280" s="8"/>
     </row>
     <row r="281" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A281" s="4"/>
-      <c r="B281" s="4"/>
+      <c r="A281" s="13"/>
+      <c r="B281" s="8"/>
     </row>
     <row r="282" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A282" s="4"/>
-      <c r="B282" s="4"/>
+      <c r="A282" s="13"/>
+      <c r="B282" s="8"/>
     </row>
     <row r="283" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A283" s="4"/>
-      <c r="B283" s="4"/>
+      <c r="A283" s="13"/>
+      <c r="B283" s="8"/>
     </row>
     <row r="284" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A284" s="4"/>
-      <c r="B284" s="4"/>
+      <c r="A284" s="13"/>
+      <c r="B284" s="8"/>
     </row>
     <row r="285" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A285" s="4"/>
-      <c r="B285" s="4"/>
+      <c r="A285" s="13"/>
+      <c r="B285" s="8"/>
     </row>
     <row r="286" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A286" s="4"/>
-      <c r="B286" s="4"/>
+      <c r="A286" s="13"/>
+      <c r="B286" s="8"/>
     </row>
     <row r="287" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A287" s="4"/>
-      <c r="B287" s="4"/>
+      <c r="A287" s="13"/>
+      <c r="B287" s="8"/>
     </row>
     <row r="288" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A288" s="4"/>
-      <c r="B288" s="4"/>
+      <c r="A288" s="13"/>
+      <c r="B288" s="8"/>
     </row>
     <row r="289" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A289" s="4"/>
-      <c r="B289" s="4"/>
+      <c r="A289" s="13"/>
+      <c r="B289" s="8"/>
     </row>
     <row r="290" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A290" s="4"/>
-      <c r="B290" s="4"/>
+      <c r="A290" s="13"/>
+      <c r="B290" s="8"/>
     </row>
     <row r="291" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A291" s="4"/>
-      <c r="B291" s="4"/>
+      <c r="A291" s="13"/>
+      <c r="B291" s="8"/>
     </row>
     <row r="292" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A292" s="4"/>
-      <c r="B292" s="4"/>
+      <c r="A292" s="13"/>
+      <c r="B292" s="8"/>
     </row>
     <row r="293" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A293" s="4"/>
-      <c r="B293" s="4"/>
+      <c r="A293" s="13"/>
+      <c r="B293" s="8"/>
     </row>
     <row r="294" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A294" s="4"/>
-      <c r="B294" s="4"/>
+      <c r="A294" s="13"/>
+      <c r="B294" s="8"/>
     </row>
     <row r="295" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A295" s="4"/>
-      <c r="B295" s="4"/>
+      <c r="A295" s="13"/>
+      <c r="B295" s="8"/>
     </row>
     <row r="296" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A296" s="4"/>
-      <c r="B296" s="4"/>
+      <c r="A296" s="13"/>
+      <c r="B296" s="8"/>
     </row>
     <row r="297" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A297" s="4"/>
-      <c r="B297" s="4"/>
+      <c r="A297" s="13"/>
+      <c r="B297" s="8"/>
     </row>
     <row r="298" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A298" s="4"/>
-      <c r="B298" s="4"/>
+      <c r="A298" s="13"/>
+      <c r="B298" s="8"/>
     </row>
     <row r="299" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A299" s="4"/>
-      <c r="B299" s="4"/>
+      <c r="A299" s="13"/>
+      <c r="B299" s="8"/>
     </row>
     <row r="300" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A300" s="4"/>
-      <c r="B300" s="4"/>
+      <c r="A300" s="13"/>
+      <c r="B300" s="8"/>
     </row>
     <row r="301" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A301" s="4"/>
-      <c r="B301" s="4"/>
+      <c r="A301" s="13"/>
+      <c r="B301" s="8"/>
     </row>
     <row r="302" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A302" s="4"/>
-      <c r="B302" s="4"/>
+      <c r="A302" s="13"/>
+      <c r="B302" s="8"/>
     </row>
     <row r="303" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A303" s="4"/>
-      <c r="B303" s="4"/>
+      <c r="A303" s="13"/>
+      <c r="B303" s="8"/>
     </row>
     <row r="304" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A304" s="4"/>
-      <c r="B304" s="4"/>
+      <c r="A304" s="13"/>
+      <c r="B304" s="8"/>
     </row>
     <row r="305" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="4"/>
-      <c r="B305" s="4"/>
+      <c r="A305" s="13"/>
+      <c r="B305" s="8"/>
     </row>
     <row r="306" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A306" s="4"/>
-      <c r="B306" s="4"/>
+      <c r="A306" s="13"/>
+      <c r="B306" s="8"/>
     </row>
     <row r="307" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A307" s="4"/>
-      <c r="B307" s="4"/>
+      <c r="A307" s="13"/>
+      <c r="B307" s="8"/>
     </row>
     <row r="308" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="4"/>
-      <c r="B308" s="4"/>
+      <c r="B308" s="8"/>
     </row>
     <row r="309" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="4"/>
@@ -5175,11 +5199,14 @@
       <c r="B1001" s="4"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B13:B308" xr:uid="{9B14A16A-4AE7-6348-B785-77E0376DBC39}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Index!$A$2:$A$3</xm:f>
@@ -5187,7 +5214,13 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B12:B108 A9:A11</xm:sqref>
+          <xm:sqref>A9:A11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2951BA3B-C7F3-1545-966D-2BEF1FC113E7}">
+          <x14:formula1>
+            <xm:f>Index!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A12:A307</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>